<commit_message>
Added new hampton tests
</commit_message>
<xml_diff>
--- a/AccelliTrackUni/Data/QuestByNumber.xlsx
+++ b/AccelliTrackUni/Data/QuestByNumber.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9405" activeTab="4"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9405" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ManageTests" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Check</t>
   </si>
@@ -97,19 +97,32 @@
   </si>
   <si>
     <t>Expected checkmark</t>
+  </si>
+  <si>
+    <t>Expected Service</t>
+  </si>
+  <si>
+    <t>Expected need</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -677,12 +690,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,9 +706,11 @@
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,10 +732,16 @@
       <c r="G1" t="s">
         <v>21</v>
       </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -749,8 +770,8 @@
   <sheetPr codeName="Лист4"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +875,7 @@
   <sheetPr codeName="Лист5"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>